<commit_message>
Track Builds w/ Switches!
</commit_message>
<xml_diff>
--- a/resources/Sample_Track_File2.xlsx
+++ b/resources/Sample_Track_File2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justc\Documents\School Stuff\Fall_2019\COE1186\Code\COE1186\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29057F43-597A-43F6-A834-79EAEBF37887}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ADA1EF-0938-40B7-B2FE-38E854FFBCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Vehicle Data 1" sheetId="5" r:id="rId5"/>
     <sheet name="Vehicle Data 2" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Red Line'!$K$1:$K$156</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="79">
   <si>
     <t>Block Number</t>
   </si>
@@ -101,9 +104,6 @@
     <t>I</t>
   </si>
   <si>
-    <t>STATION</t>
-  </si>
-  <si>
     <t>J</t>
   </si>
   <si>
@@ -140,13 +140,7 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>ELEVATION (M)</t>
-  </si>
-  <si>
-    <t>CUMALTIVE ELEVATION (M)</t>
   </si>
   <si>
     <t>STATION;     STEEL PLAZA; UNDERGROUND</t>
@@ -224,9 +218,6 @@
     <t>SWITCH (12-13; 1-13)</t>
   </si>
   <si>
-    <t>SWITCH (28-30; 28-150)</t>
-  </si>
-  <si>
     <t>SWITCH TO YARD (57-yard)</t>
   </si>
   <si>
@@ -276,6 +267,12 @@
   </si>
   <si>
     <t>CUMULATIVE ELEVATION (M)</t>
+  </si>
+  <si>
+    <t>SWITCH (28-29; 28-150)</t>
+  </si>
+  <si>
+    <t>STATION; NONAME</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1045,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1079,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
@@ -1115,16 +1112,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -1148,7 +1145,7 @@
         <v>40</v>
       </c>
       <c r="I2" s="12">
-        <f>E2*D2/100</f>
+        <f t="shared" ref="I2:I33" si="0">E2*D2/100</f>
         <v>0.25</v>
       </c>
       <c r="J2" s="12">
@@ -1178,18 +1175,18 @@
         <v>40</v>
       </c>
       <c r="I3" s="12">
-        <f t="shared" ref="I3:I66" si="0">E3*D3/100</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
       <c r="J3" s="12">
-        <f>I3+J2</f>
+        <f t="shared" ref="J3:J34" si="1">I3+J2</f>
         <v>0.75</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="str">
-        <f t="shared" ref="A4:A70" si="1">A3</f>
+        <f t="shared" ref="A4:A70" si="2">A3</f>
         <v>Red</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1212,14 +1209,14 @@
         <v>0.75</v>
       </c>
       <c r="J4" s="12">
-        <f t="shared" ref="J4:J67" si="2">I4+J3</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1242,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="J5" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1271,13 +1268,13 @@
         <v>0.75</v>
       </c>
       <c r="J6" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.25</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1300,13 +1297,13 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1325,20 +1322,20 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
         <v>0.375</v>
       </c>
       <c r="J8" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.125</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1361,13 +1358,13 @@
         <v>0</v>
       </c>
       <c r="J9" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.125</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1386,20 +1383,20 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.125</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1422,13 +1419,13 @@
         <v>0</v>
       </c>
       <c r="J11" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.125</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1451,13 +1448,13 @@
         <v>-0.375</v>
       </c>
       <c r="J12" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1480,13 +1477,13 @@
         <v>-0.75</v>
       </c>
       <c r="J13" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1509,13 +1506,13 @@
         <v>-1.4</v>
       </c>
       <c r="J14" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1538,13 +1535,13 @@
         <v>-0.75</v>
       </c>
       <c r="J15" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.85000000000000009</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1563,20 +1560,20 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
         <v>-0.6</v>
       </c>
       <c r="J16" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.25000000000000011</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1595,20 +1592,20 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
         <v>-0.25</v>
       </c>
       <c r="J17" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1627,17 +1624,17 @@
         <v>55</v>
       </c>
       <c r="I18" s="12">
-        <f>E18*D18/100</f>
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="J18" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1661,13 +1658,13 @@
         <v>-0.24099999999999999</v>
       </c>
       <c r="J19" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1690,13 +1687,13 @@
         <v>0</v>
       </c>
       <c r="J20" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1719,13 +1716,13 @@
         <v>0</v>
       </c>
       <c r="J21" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1744,20 +1741,20 @@
         <v>55</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J22" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1780,13 +1777,13 @@
         <v>0</v>
       </c>
       <c r="J23" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1809,13 +1806,13 @@
         <v>0</v>
       </c>
       <c r="J24" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1834,20 +1831,20 @@
         <v>70</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J25" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1866,20 +1863,20 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J26" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1898,20 +1895,20 @@
         <v>70</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I27" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J27" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1930,20 +1927,20 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J28" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1962,20 +1959,20 @@
         <v>70</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I29" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J29" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1994,20 +1991,20 @@
         <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I30" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J30" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2026,20 +2023,20 @@
         <v>70</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I31" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J31" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2058,20 +2055,20 @@
         <v>70</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I32" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J32" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2090,20 +2087,20 @@
         <v>70</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J33" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2122,20 +2119,20 @@
         <v>70</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I34" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I34:I65" si="3">E34*D34/100</f>
         <v>0</v>
       </c>
       <c r="J34" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2154,20 +2151,20 @@
         <v>70</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I35" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J35" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J35:J66" si="4">I35+J34</f>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2186,20 +2183,20 @@
         <v>70</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I36" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J36" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2218,14 +2215,14 @@
         <v>70</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I37" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J37" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
@@ -2250,20 +2247,20 @@
         <v>70</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I38" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J38" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2282,20 +2279,20 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I39" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J39" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2314,20 +2311,20 @@
         <v>70</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I40" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J40" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2346,20 +2343,20 @@
         <v>70</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I41" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J41" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2378,20 +2375,20 @@
         <v>70</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I42" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J42" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2410,20 +2407,20 @@
         <v>70</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I43" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J43" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2442,20 +2439,20 @@
         <v>70</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I44" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J44" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2474,20 +2471,20 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I45" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J45" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2506,20 +2503,20 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="I46" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J46" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -2538,20 +2535,20 @@
         <v>70</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I47" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J47" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -2570,20 +2567,20 @@
         <v>70</v>
       </c>
       <c r="G48" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I48" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J48" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -2602,24 +2599,24 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I49" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J49" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" s="3">
         <v>49</v>
@@ -2634,21 +2631,21 @@
         <v>60</v>
       </c>
       <c r="I50" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J50" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" s="5">
         <v>50</v>
@@ -2663,21 +2660,21 @@
         <v>60</v>
       </c>
       <c r="I51" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J51" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C52" s="3">
         <v>51</v>
@@ -2692,21 +2689,21 @@
         <v>55</v>
       </c>
       <c r="I52" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J52" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C53" s="3">
         <v>52</v>
@@ -2721,24 +2718,24 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I53" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J53" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" s="5">
         <v>53</v>
@@ -2753,21 +2750,21 @@
         <v>55</v>
       </c>
       <c r="I54" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J54" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="3">
         <v>54</v>
@@ -2782,21 +2779,21 @@
         <v>55</v>
       </c>
       <c r="I55" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J55" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C56" s="3">
         <v>55</v>
@@ -2811,21 +2808,21 @@
         <v>55</v>
       </c>
       <c r="I56" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.375</v>
       </c>
       <c r="J56" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.8660000000000001</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C57" s="5">
         <v>56</v>
@@ -2840,21 +2837,21 @@
         <v>55</v>
       </c>
       <c r="I57" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.375</v>
       </c>
       <c r="J57" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.4910000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C58" s="3">
         <v>57</v>
@@ -2869,21 +2866,21 @@
         <v>55</v>
       </c>
       <c r="I58" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.375</v>
       </c>
       <c r="J58" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.1160000000000001</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C59" s="3">
         <v>58</v>
@@ -2898,21 +2895,21 @@
         <v>55</v>
       </c>
       <c r="I59" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
       <c r="J59" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.6339999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="5">
         <v>59</v>
@@ -2927,21 +2924,21 @@
         <v>55</v>
       </c>
       <c r="I60" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0.375</v>
       </c>
       <c r="J60" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0089999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C61" s="3">
         <v>60</v>
@@ -2956,24 +2953,24 @@
         <v>55</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I61" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J61" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.0089999999999999</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C62" s="3">
         <v>61</v>
@@ -2988,21 +2985,21 @@
         <v>55</v>
       </c>
       <c r="I62" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.375</v>
       </c>
       <c r="J62" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.6339999999999999</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C63" s="5">
         <v>62</v>
@@ -3017,21 +3014,21 @@
         <v>55</v>
       </c>
       <c r="I63" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="J63" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.1160000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C64" s="3">
         <v>63</v>
@@ -3046,21 +3043,21 @@
         <v>55</v>
       </c>
       <c r="I64" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="J64" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-0.8660000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C65" s="3">
         <v>64</v>
@@ -3075,21 +3072,21 @@
         <v>55</v>
       </c>
       <c r="I65" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-0.375</v>
       </c>
       <c r="J65" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="5">
         <v>65</v>
@@ -3104,21 +3101,21 @@
         <v>55</v>
       </c>
       <c r="I66" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I66:I77" si="5">E66*D66/100</f>
         <v>0</v>
       </c>
       <c r="J66" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C67" s="3">
         <v>66</v>
@@ -3133,21 +3130,21 @@
         <v>55</v>
       </c>
       <c r="I67" s="12">
-        <f t="shared" ref="I67:I77" si="3">E67*D67/100</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J67" s="12">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="J67:J98" si="6">I67+J66</f>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C68" s="3">
         <v>67</v>
@@ -3162,24 +3159,24 @@
         <v>55</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I68" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J68" s="12">
-        <f t="shared" ref="J68:J77" si="4">I68+J67</f>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" s="5">
         <v>68</v>
@@ -3194,24 +3191,24 @@
         <v>55</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I69" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J69" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Red</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C70" s="3">
         <v>69</v>
@@ -3226,24 +3223,24 @@
         <v>55</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I70" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J70" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="str">
-        <f t="shared" ref="A71:A134" si="5">A70</f>
+        <f t="shared" ref="A71:A77" si="7">A70</f>
         <v>Red</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C71" s="3">
         <v>70</v>
@@ -3258,24 +3255,24 @@
         <v>55</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I71" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J71" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C72" s="5">
         <v>71</v>
@@ -3290,24 +3287,24 @@
         <v>55</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I72" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J72" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C73" s="3">
         <v>72</v>
@@ -3322,24 +3319,24 @@
         <v>55</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I73" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J73" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C74" s="3">
         <v>73</v>
@@ -3354,24 +3351,24 @@
         <v>55</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I74" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J74" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C75" s="5">
         <v>74</v>
@@ -3386,24 +3383,24 @@
         <v>55</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I75" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J75" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C76" s="3">
         <v>75</v>
@@ -3418,24 +3415,24 @@
         <v>55</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I76" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J76" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>Red</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C77" s="3">
         <v>76</v>
@@ -3450,556 +3447,252 @@
         <v>55</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I77" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J77" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-1.2410000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A80" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96" s="5"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="5"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="5"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101" s="5"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102" s="5"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104" s="5"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105" s="5"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106" s="5"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107" s="5"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108" s="5"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109" s="5"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110" s="5"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111" s="5"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112" s="5"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113" s="5"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114" s="5"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115" s="5"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116" s="5"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117" s="5"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A118" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118" s="5"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A119" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119" s="5"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A120" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120" s="5"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121" s="5"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A122" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122" s="5"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A123" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C123" s="5"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C124" s="5"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A125" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C125" s="5"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A126" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C126" s="5"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A127" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C127" s="5"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A128" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C128" s="5"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C129" s="5"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C130" s="5"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C131" s="5"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C132" s="5"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C133" s="5"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C134" s="5"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="3" t="str">
-        <f t="shared" ref="A135:A154" si="6">A134</f>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C135" s="5"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A136" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C136" s="5"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A137" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C137" s="5"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A138" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C138" s="5"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A139" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C139" s="5"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A140" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C140" s="5"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A141" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C141" s="5"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A142" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C142" s="5"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A143" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C143" s="5"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A144" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C144" s="5"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A145" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C145" s="5"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A146" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C146" s="5"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A147" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C147" s="5"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A148" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C148" s="5"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A149" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C149" s="5"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A150" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C150" s="5"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A151" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C151" s="5"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A152" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C152" s="5"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C153" s="5"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A154" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve"> </v>
-      </c>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C154" s="5"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K1:K155">
+    <sortCondition descending="1" ref="K1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4009,9 +3702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4045,16 +3738,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -4108,7 +3801,7 @@
         <v>55</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I66" si="0">E3*D3/100</f>
@@ -4257,7 +3950,6 @@
       <c r="F8" s="3">
         <v>55</v>
       </c>
-      <c r="G8" s="11"/>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4317,7 +4009,7 @@
         <v>55</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
@@ -4407,7 +4099,7 @@
         <v>55</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
@@ -4526,7 +4218,7 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
@@ -4616,7 +4308,7 @@
         <v>60</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
@@ -4706,7 +4398,7 @@
         <v>70</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I23" s="3">
         <f t="shared" si="0"/>
@@ -4912,7 +4604,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
@@ -4973,7 +4665,7 @@
         <v>70</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I32" s="3">
         <f t="shared" si="0"/>
@@ -5121,7 +4813,7 @@
         <v>70</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I37" s="3">
         <f t="shared" si="0"/>
@@ -5153,7 +4845,7 @@
         <v>70</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I38" s="3">
         <f t="shared" si="0"/>
@@ -5185,7 +4877,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I39" s="3">
         <f t="shared" si="0"/>
@@ -5217,7 +4909,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I40" s="3">
         <f t="shared" si="0"/>
@@ -5249,7 +4941,7 @@
         <v>70</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I41" s="3">
         <f t="shared" si="0"/>
@@ -5281,7 +4973,7 @@
         <v>70</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I42" s="3">
         <f t="shared" si="0"/>
@@ -5313,7 +5005,7 @@
         <v>70</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I43" s="3">
         <f t="shared" si="0"/>
@@ -5345,7 +5037,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I44" s="3">
         <f t="shared" si="0"/>
@@ -5377,7 +5069,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I45" s="3">
         <f t="shared" si="0"/>
@@ -5409,7 +5101,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I46" s="3">
         <f t="shared" si="0"/>
@@ -5441,7 +5133,7 @@
         <v>70</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I47" s="3">
         <f t="shared" si="0"/>
@@ -5473,7 +5165,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I48" s="3">
         <f t="shared" si="0"/>
@@ -5505,7 +5197,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I49" s="3">
         <f t="shared" si="0"/>
@@ -5537,7 +5229,7 @@
         <v>70</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I50" s="3">
         <f t="shared" si="0"/>
@@ -5569,7 +5261,7 @@
         <v>70</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I51" s="3">
         <f t="shared" si="0"/>
@@ -5601,7 +5293,7 @@
         <v>70</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I52" s="3">
         <f t="shared" si="0"/>
@@ -5633,7 +5325,7 @@
         <v>70</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I53" s="3">
         <f t="shared" si="0"/>
@@ -5665,7 +5357,7 @@
         <v>70</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I54" s="3">
         <f t="shared" si="0"/>
@@ -5697,7 +5389,7 @@
         <v>70</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I55" s="3">
         <f t="shared" si="0"/>
@@ -5729,7 +5421,7 @@
         <v>70</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I56" s="3">
         <f t="shared" si="0"/>
@@ -5761,7 +5453,7 @@
         <v>70</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I57" s="3">
         <f t="shared" si="0"/>
@@ -5793,7 +5485,7 @@
         <v>70</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I58" s="3">
         <f t="shared" si="0"/>
@@ -5810,7 +5502,7 @@
         <v>Green</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C59" s="3">
         <v>58</v>
@@ -5825,7 +5517,7 @@
         <v>60</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I59" s="3">
         <f t="shared" si="0"/>
@@ -5842,7 +5534,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60" s="5">
         <v>59</v>
@@ -5871,7 +5563,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C61" s="3">
         <v>60</v>
@@ -5900,7 +5592,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C62" s="3">
         <v>61</v>
@@ -5929,7 +5621,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C63" s="5">
         <v>62</v>
@@ -5944,7 +5636,7 @@
         <v>60</v>
       </c>
       <c r="G63" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
@@ -5961,7 +5653,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C64" s="3">
         <v>63</v>
@@ -5990,7 +5682,7 @@
         <v>Green</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C65" s="3">
         <v>64</v>
@@ -6019,7 +5711,7 @@
         <v>Green</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C66" s="5">
         <v>65</v>
@@ -6034,7 +5726,7 @@
         <v>70</v>
       </c>
       <c r="G66" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I66" s="3">
         <f t="shared" si="0"/>
@@ -6051,7 +5743,7 @@
         <v>Green</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C67" s="3">
         <v>66</v>
@@ -6080,7 +5772,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C68" s="3">
         <v>67</v>
@@ -6109,7 +5801,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C69" s="5">
         <v>68</v>
@@ -6138,7 +5830,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C70" s="3">
         <v>69</v>
@@ -6167,7 +5859,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C71" s="3">
         <v>70</v>
@@ -6196,7 +5888,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C72" s="5">
         <v>71</v>
@@ -6225,7 +5917,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C73" s="3">
         <v>72</v>
@@ -6254,7 +5946,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C74" s="3">
         <v>73</v>
@@ -6269,7 +5961,7 @@
         <v>60</v>
       </c>
       <c r="G74" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I74" s="3">
         <f t="shared" si="3"/>
@@ -6286,7 +5978,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C75" s="5">
         <v>74</v>
@@ -6315,7 +6007,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C76" s="3">
         <v>75</v>
@@ -6344,7 +6036,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C77" s="3">
         <v>76</v>
@@ -6359,7 +6051,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
@@ -6376,7 +6068,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C78" s="3">
         <v>77</v>
@@ -6391,7 +6083,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="6">E78*D78/100</f>
@@ -6408,7 +6100,7 @@
         <v>Green</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C79" s="5">
         <v>78</v>
@@ -6437,7 +6129,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C80" s="3">
         <v>79</v>
@@ -6466,7 +6158,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C81" s="3">
         <v>80</v>
@@ -6495,7 +6187,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C82" s="3">
         <v>81</v>
@@ -6524,7 +6216,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C83" s="5">
         <v>82</v>
@@ -6553,7 +6245,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C84" s="3">
         <v>83</v>
@@ -6582,7 +6274,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C85" s="3">
         <v>84</v>
@@ -6611,7 +6303,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C86" s="3">
         <v>85</v>
@@ -6640,7 +6332,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C87" s="5">
         <v>86</v>
@@ -6655,7 +6347,7 @@
         <v>55</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I87" s="3">
         <f t="shared" si="6"/>
@@ -6672,7 +6364,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C88" s="3">
         <v>87</v>
@@ -6701,7 +6393,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C89" s="3">
         <v>88</v>
@@ -6716,7 +6408,7 @@
         <v>55</v>
       </c>
       <c r="G89" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I89" s="3">
         <f t="shared" si="6"/>
@@ -6733,7 +6425,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C90" s="3">
         <v>89</v>
@@ -6762,7 +6454,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C91" s="5">
         <v>90</v>
@@ -6791,7 +6483,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C92" s="3">
         <v>91</v>
@@ -6820,7 +6512,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C93" s="3">
         <v>92</v>
@@ -6849,7 +6541,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C94" s="3">
         <v>93</v>
@@ -6878,7 +6570,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C95" s="5">
         <v>94</v>
@@ -6907,7 +6599,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C96" s="3">
         <v>95</v>
@@ -6936,7 +6628,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C97" s="3">
         <v>96</v>
@@ -6951,7 +6643,7 @@
         <v>55</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I97" s="3">
         <f t="shared" si="6"/>
@@ -6968,7 +6660,7 @@
         <v>Green</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C98" s="3">
         <v>97</v>
@@ -6997,7 +6689,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C99" s="5">
         <v>98</v>
@@ -7026,7 +6718,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C100" s="3">
         <v>99</v>
@@ -7055,7 +6747,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C101" s="3">
         <v>100</v>
@@ -7084,7 +6776,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C102" s="3">
         <v>101</v>
@@ -7113,7 +6805,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C103" s="5">
         <v>102</v>
@@ -7142,7 +6834,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C104" s="3">
         <v>103</v>
@@ -7171,7 +6863,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C105" s="3">
         <v>104</v>
@@ -7200,7 +6892,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C106" s="3">
         <v>105</v>
@@ -7233,7 +6925,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C107" s="5">
         <v>106</v>
@@ -7262,7 +6954,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C108" s="3">
         <v>107</v>
@@ -7291,7 +6983,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C109" s="3">
         <v>108</v>
@@ -7320,7 +7012,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C110" s="3">
         <v>109</v>
@@ -7349,7 +7041,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C111" s="5">
         <v>110</v>
@@ -7378,7 +7070,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C112" s="3">
         <v>111</v>
@@ -7407,7 +7099,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C113" s="3">
         <v>112</v>
@@ -7436,7 +7128,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C114" s="3">
         <v>113</v>
@@ -7465,7 +7157,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C115" s="5">
         <v>114</v>
@@ -7499,7 +7191,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C116" s="3">
         <v>115</v>
@@ -7528,7 +7220,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C117" s="3">
         <v>116</v>
@@ -7557,7 +7249,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C118" s="3">
         <v>117</v>
@@ -7586,7 +7278,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C119" s="5">
         <v>118</v>
@@ -7615,7 +7307,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C120" s="3">
         <v>119</v>
@@ -7644,7 +7336,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C121" s="3">
         <v>120</v>
@@ -7673,7 +7365,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C122" s="3">
         <v>121</v>
@@ -7702,7 +7394,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C123" s="5">
         <v>122</v>
@@ -7717,7 +7409,7 @@
         <v>70</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I123" s="3">
         <f t="shared" si="8"/>
@@ -7734,7 +7426,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C124" s="3">
         <v>123</v>
@@ -7767,7 +7459,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C125" s="3">
         <v>124</v>
@@ -7782,7 +7474,7 @@
         <v>70</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I125" s="3">
         <f t="shared" si="8"/>
@@ -7799,7 +7491,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C126" s="3">
         <v>125</v>
@@ -7814,7 +7506,7 @@
         <v>70</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I126" s="3">
         <f t="shared" si="8"/>
@@ -7831,7 +7523,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C127" s="5">
         <v>126</v>
@@ -7846,7 +7538,7 @@
         <v>70</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I127" s="3">
         <f t="shared" si="8"/>
@@ -7863,7 +7555,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C128" s="3">
         <v>127</v>
@@ -7878,7 +7570,7 @@
         <v>70</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I128" s="3">
         <f t="shared" si="8"/>
@@ -7895,7 +7587,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C129" s="3">
         <v>128</v>
@@ -7910,7 +7602,7 @@
         <v>70</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I129" s="3">
         <f t="shared" si="8"/>
@@ -7927,7 +7619,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C130" s="3">
         <v>129</v>
@@ -7942,7 +7634,7 @@
         <v>70</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I130" s="3">
         <f t="shared" si="8"/>
@@ -7959,7 +7651,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C131" s="5">
         <v>130</v>
@@ -7974,7 +7666,7 @@
         <v>70</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I131" s="3">
         <f t="shared" si="8"/>
@@ -7991,7 +7683,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C132" s="3">
         <v>131</v>
@@ -8006,7 +7698,7 @@
         <v>70</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I132" s="3">
         <f t="shared" si="8"/>
@@ -8023,7 +7715,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C133" s="3">
         <v>132</v>
@@ -8056,7 +7748,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C134" s="3">
         <v>133</v>
@@ -8071,7 +7763,7 @@
         <v>70</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I134" s="3">
         <f t="shared" si="8"/>
@@ -8088,7 +7780,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C135" s="5">
         <v>134</v>
@@ -8103,7 +7795,7 @@
         <v>70</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I135" s="3">
         <f t="shared" si="8"/>
@@ -8120,7 +7812,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C136" s="3">
         <v>135</v>
@@ -8135,7 +7827,7 @@
         <v>70</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I136" s="3">
         <f t="shared" si="8"/>
@@ -8152,7 +7844,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C137" s="3">
         <v>136</v>
@@ -8167,7 +7859,7 @@
         <v>70</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I137" s="3">
         <f t="shared" si="8"/>
@@ -8184,7 +7876,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C138" s="3">
         <v>137</v>
@@ -8199,7 +7891,7 @@
         <v>70</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I138" s="3">
         <f t="shared" si="8"/>
@@ -8216,7 +7908,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C139" s="5">
         <v>138</v>
@@ -8231,7 +7923,7 @@
         <v>70</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I139" s="3">
         <f t="shared" si="8"/>
@@ -8248,7 +7940,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C140" s="3">
         <v>139</v>
@@ -8263,7 +7955,7 @@
         <v>70</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I140" s="3">
         <f t="shared" si="8"/>
@@ -8280,7 +7972,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C141" s="3">
         <v>140</v>
@@ -8295,7 +7987,7 @@
         <v>70</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I141" s="3">
         <f t="shared" si="8"/>
@@ -8312,7 +8004,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C142" s="3">
         <v>141</v>
@@ -8345,7 +8037,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C143" s="5">
         <v>142</v>
@@ -8360,7 +8052,7 @@
         <v>70</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I143" s="3">
         <f t="shared" si="8"/>
@@ -8377,7 +8069,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C144" s="3">
         <v>143</v>
@@ -8392,7 +8084,7 @@
         <v>70</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I144" s="3">
         <f t="shared" si="8"/>
@@ -8409,7 +8101,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C145" s="3">
         <v>144</v>
@@ -8438,7 +8130,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C146" s="3">
         <v>145</v>
@@ -8467,7 +8159,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C147" s="5">
         <v>146</v>
@@ -8496,7 +8188,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C148" s="3">
         <v>147</v>
@@ -8525,7 +8217,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C149" s="3">
         <v>148</v>
@@ -8555,7 +8247,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C150" s="3">
         <v>149</v>
@@ -8584,7 +8276,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C151" s="5">
         <v>150</v>
@@ -8616,7 +8308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Verified correct track building
</commit_message>
<xml_diff>
--- a/resources/Sample_Track_File2.xlsx
+++ b/resources/Sample_Track_File2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justc\Documents\School Stuff\Fall_2019\COE1186\Code\COE1186\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ADA1EF-0938-40B7-B2FE-38E854FFBCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B7CC35-4098-41B6-996B-1A83CE13F1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
     <t>SWITCH FROM YARD (Yard-63)</t>
   </si>
   <si>
-    <t>SWITCH (76-77;77-101)</t>
-  </si>
-  <si>
     <t>STATION; MT LEBANON</t>
   </si>
   <si>
@@ -273,6 +270,9 @@
   </si>
   <si>
     <t>STATION; NONAME</t>
+  </si>
+  <si>
+    <t>SWITCH (76-77; 77-101)</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1121,7 +1121,7 @@
         <v>34</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -1322,7 +1322,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
@@ -1383,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
@@ -1592,7 +1592,7 @@
         <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I17" s="12">
         <f t="shared" si="0"/>
@@ -1863,7 +1863,7 @@
         <v>70</v>
       </c>
       <c r="G26" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I26" s="12">
         <f t="shared" si="0"/>
@@ -1927,7 +1927,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I28" s="12">
         <f t="shared" si="0"/>
@@ -2087,7 +2087,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
@@ -2279,7 +2279,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I39" s="12">
         <f t="shared" si="3"/>
@@ -2439,7 +2439,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I44" s="12">
         <f t="shared" si="3"/>
@@ -2503,7 +2503,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I46" s="12">
         <f t="shared" si="3"/>
@@ -2718,7 +2718,7 @@
         <v>55</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I53" s="12">
         <f t="shared" si="3"/>
@@ -3703,8 +3703,8 @@
   <dimension ref="A1:L151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3747,7 +3747,7 @@
         <v>34</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -4218,7 +4218,7 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
@@ -4604,7 +4604,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
@@ -6051,7 +6051,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
@@ -6083,7 +6083,7 @@
         <v>70</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I78" s="3">
         <f t="shared" ref="I78:I109" si="6">E78*D78/100</f>
@@ -6347,7 +6347,7 @@
         <v>55</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I87" s="3">
         <f t="shared" si="6"/>
@@ -8308,7 +8308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added debugging statement, pushed hunk I forgot earlier
</commit_message>
<xml_diff>
--- a/resources/Sample_Track_File2.xlsx
+++ b/resources/Sample_Track_File2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justc\Documents\School Stuff\Fall_2019\COE1186\Code\COE1186\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B7CC35-4098-41B6-996B-1A83CE13F1D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B9C76A-4EAB-4AC9-9026-2E120FE6C9BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -269,10 +269,10 @@
     <t>SWITCH (28-29; 28-150)</t>
   </si>
   <si>
-    <t>STATION; NONAME</t>
+    <t>SWITCH (76-77; 77-101)</t>
   </si>
   <si>
-    <t>SWITCH (76-77; 77-101)</t>
+    <t>STATION; GRANT ST</t>
   </si>
 </sst>
 </file>
@@ -436,13 +436,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>380999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>28989</xdr:rowOff>
     </xdr:to>
@@ -468,8 +468,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="0" y="579119"/>
-          <a:ext cx="6042660" cy="7770910"/>
+          <a:off x="76200" y="577849"/>
+          <a:ext cx="6042660" cy="7814090"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1076,9 +1076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
       <c r="J67" s="12">
-        <f t="shared" ref="J67:J98" si="6">I67+J66</f>
+        <f t="shared" ref="J67:J77" si="6">I67+J66</f>
         <v>-1.2410000000000001</v>
       </c>
     </row>
@@ -3702,9 +3702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L151"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G77" sqref="G77"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4218,7 +4218,7 @@
         <v>70</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
@@ -6051,7 +6051,7 @@
         <v>60</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I77" s="3">
         <f t="shared" si="3"/>
@@ -8308,8 +8308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView topLeftCell="A4" zoomScale="56" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>